<commit_message>
update data source server CapabilityStatement
</commit_message>
<xml_diff>
--- a/input/resources-spreadsheet/data-source-server.xlsx
+++ b/input/resources-spreadsheet/data-source-server.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/Davinci-CDEX/input/resources-spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{476122B6-7156-C944-A72E-82607AB515B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E532F9EC-2F96-5842-A4F1-EDFF61EC9C82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-900" yWindow="960" windowWidth="28800" windowHeight="17540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3280" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="155">
   <si>
     <t>Element</t>
   </si>
@@ -369,10 +369,171 @@
     <t>data-source-server</t>
   </si>
   <si>
-    <t>0.2.0</t>
-  </si>
-  <si>
     <t>server</t>
+  </si>
+  <si>
+    <t>HRex Task Data Request Profile</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Required resource type to fetch Clinical Information from data source</t>
+  </si>
+  <si>
+    <t>Subscription</t>
+  </si>
+  <si>
+    <t>Required resource type to subscribe to data source</t>
+  </si>
+  <si>
+    <t>conf_Subscription</t>
+  </si>
+  <si>
+    <t>doc_Subscription</t>
+  </si>
+  <si>
+    <t>conf_Task</t>
+  </si>
+  <si>
+    <t>doc_Task</t>
+  </si>
+  <si>
+    <t>transaction</t>
+  </si>
+  <si>
+    <t>batch</t>
+  </si>
+  <si>
+    <t>search-system</t>
+  </si>
+  <si>
+    <t>history-system</t>
+  </si>
+  <si>
+    <t>CDex Task Data Request Profile</t>
+  </si>
+  <si>
+    <t>!http://hl7.org/fhir/us/davinci-hrex/StructureDefinition/hrex-task-data-request</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-cdex/StructureDefinition/cdex-task-data-request</t>
+  </si>
+  <si>
+    <t>This CapabilityStatement describes the expected capabilities of a Da Vinci CDex Data Source (often an EHR) in *Server* mode when responding to a Data Consumer (often a Payer)  during a clinical data exchange. This includes the following interactions:
+1. Responding to a FHIR RestFul Query for Clinical Data 
+1. Responding to a POST of a  Task resource representing a request for clinical data
+1. Responding to a POST of a  Subscription  resource
+1. Responding to polling of a Task resource</t>
+  </si>
+  <si>
+    <t>HL7 FHIR® US Core Implementation Guide STU3 Release 3.1.1</t>
+  </si>
+  <si>
+    <t>Da Vinci Health Record Exchange (HRex) 0.2.0 - STU R1 - 2nd ballot</t>
+  </si>
+  <si>
+    <t>/users/ehaas/Documents/FHIR/Davinci-CDEX/input/</t>
+  </si>
+  <si>
+    <t>/users/ehaas/Documents/FHIR/Davinci-CDEX/output/</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-hrex/ImplementationGuide/hl7.fhir.us.davinci-hrex|0.2.0</t>
+  </si>
+  <si>
+    <t>imports</t>
+  </si>
+  <si>
+    <t>instantiates</t>
+  </si>
+  <si>
+    <t>canonical</t>
+  </si>
+  <si>
+    <t>US Core Server CapabilityStatement</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/CapabilityStatement/us-core-server</t>
+  </si>
+  <si>
+    <t>format</t>
+  </si>
+  <si>
+    <t>json,xml</t>
+  </si>
+  <si>
+    <t>format_conf</t>
+  </si>
+  <si>
+    <t>SHALL,SHOULD</t>
+  </si>
+  <si>
+    <t>patchFormat</t>
+  </si>
+  <si>
+    <t>patchFormat_conf</t>
+  </si>
+  <si>
+    <t>suppress_may_sps</t>
+  </si>
+  <si>
+    <t>include_conf</t>
+  </si>
+  <si>
+    <t>include</t>
+  </si>
+  <si>
+    <t>revinclude</t>
+  </si>
+  <si>
+    <t>revinclude_conf</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-hrex/2020Sep/StructureDefinition-hrex-coverage.html</t>
+  </si>
+  <si>
+    <t>HRex Coverage Profile</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-pas/StructureDefinition/profile-claim</t>
+  </si>
+  <si>
+    <t>PAS Claim</t>
+  </si>
+  <si>
+    <t>Claim</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-pas/StructureDefinition-profile-claim.html</t>
+  </si>
+  <si>
+    <t>conf_Claim</t>
+  </si>
+  <si>
+    <t>doc_Claim</t>
+  </si>
+  <si>
+    <t>Resource type to carry information regarding reason for requesting  1) attachments to support claim submission, medical necessity and other reasons for attachments between payers and providers, and 2) additional information to support prior authorization requests.</t>
+  </si>
+  <si>
+    <t>!http://hl7.org/fhir/us/davinci-hrex/StructureDefinition/hrex-coverage</t>
+  </si>
+  <si>
+    <t>* Required resource type to request and fetch clinical information from data source
+* There **SHOULD** be a reason stated in `Task.statusReason` by the Data-Source-Server when the status is updated to 'failed', 'refused', 'cancelled' or 'held'</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/index.html</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-hrex/2020Sep/index.html</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/CapabilityStatement-us-core-server.html</t>
+  </si>
+  <si>
+    <t>1.0.0</t>
   </si>
   <si>
     <t>The  Da Vinci CDex Data Source **SHALL**:
@@ -380,174 +541,20 @@
      1. Direct Query
      1. Task Based Approachs
 1. Support json source formats for all Da Vinci CDex interactions.
+1. Follow the guidelines for [Generating and Verifying Signed Resources](signatures.html) *if signatures are required*.
 1. Declare a CapabilityStatement identifying the scenarios, transactions and profiles supported.
 The  Da Vinci CDex Data Source  **SHOULD**:
 1. Support xml source formats for all Da Vinci CDex interactions.</t>
   </si>
   <si>
-    <t>1. For general security consideration refer to the [Security and Privacy Considerations](http://build.fhir.org/secpriv-module.html). 
-1. For security considerations specific to this guide refer to the Da Vinci HRex Implementation Guide section on [Security and Privacy](http://hl7.org/fhir/us/davinci-hrex/2020Sep/security.html)</t>
-  </si>
-  <si>
-    <t>HRex Task Data Request Profile</t>
-  </si>
-  <si>
-    <t>Task</t>
-  </si>
-  <si>
-    <t>Required resource type to fetch Clinical Information from data source</t>
-  </si>
-  <si>
-    <t>Subscription</t>
-  </si>
-  <si>
-    <t>Required resource type to subscribe to data source</t>
-  </si>
-  <si>
-    <t>conf_Subscription</t>
-  </si>
-  <si>
-    <t>doc_Subscription</t>
-  </si>
-  <si>
-    <t>conf_Task</t>
-  </si>
-  <si>
-    <t>doc_Task</t>
-  </si>
-  <si>
-    <t>transaction</t>
-  </si>
-  <si>
-    <t>batch</t>
-  </si>
-  <si>
-    <t>search-system</t>
-  </si>
-  <si>
-    <t>history-system</t>
-  </si>
-  <si>
-    <t>CDex Task Data Request Profile</t>
-  </si>
-  <si>
-    <t>!http://hl7.org/fhir/us/davinci-hrex/StructureDefinition/hrex-task-data-request</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-cdex/StructureDefinition/cdex-task-data-request</t>
-  </si>
-  <si>
-    <t>This CapabilityStatement describes the expected capabilities of a Da Vinci CDex Data Source (often an EHR) in *Server* mode when responding to a Data Consumer (often a Payer)  during a clinical data exchange. This includes the following interactions:
-1. Responding to a FHIR RestFul Query for Clinical Data 
-1. Responding to a POST of a  Task resource representing a request for clinical data
-1. Responding to a POST of a  Subscription  resource
-1. Responding to polling of a Task resource</t>
-  </si>
-  <si>
-    <t>HL7 FHIR® US Core Implementation Guide STU3 Release 3.1.1</t>
-  </si>
-  <si>
-    <t>Da Vinci Health Record Exchange (HRex) 0.2.0 - STU R1 - 2nd ballot</t>
-  </si>
-  <si>
-    <t>/users/ehaas/Documents/FHIR/Davinci-CDEX/input/</t>
-  </si>
-  <si>
-    <t>/users/ehaas/Documents/FHIR/Davinci-CDEX/output/</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-hrex/ImplementationGuide/hl7.fhir.us.davinci-hrex|0.2.0</t>
-  </si>
-  <si>
-    <t>imports</t>
-  </si>
-  <si>
-    <t>instantiates</t>
-  </si>
-  <si>
-    <t>canonical</t>
-  </si>
-  <si>
-    <t>US Core Server CapabilityStatement</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/CapabilityStatement/us-core-server</t>
-  </si>
-  <si>
-    <t>format</t>
-  </si>
-  <si>
-    <t>json,xml</t>
-  </si>
-  <si>
-    <t>format_conf</t>
-  </si>
-  <si>
-    <t>SHALL,SHOULD</t>
-  </si>
-  <si>
-    <t>patchFormat</t>
-  </si>
-  <si>
-    <t>patchFormat_conf</t>
-  </si>
-  <si>
-    <t>suppress_may_sps</t>
-  </si>
-  <si>
-    <t>include_conf</t>
-  </si>
-  <si>
-    <t>include</t>
-  </si>
-  <si>
-    <t>revinclude</t>
-  </si>
-  <si>
-    <t>revinclude_conf</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-hrex/2020Sep/StructureDefinition-hrex-coverage.html</t>
-  </si>
-  <si>
-    <t>HRex Coverage Profile</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-pas/StructureDefinition/profile-claim</t>
-  </si>
-  <si>
-    <t>PAS Claim</t>
-  </si>
-  <si>
-    <t>Claim</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-pas/StructureDefinition-profile-claim.html</t>
-  </si>
-  <si>
-    <t>conf_Claim</t>
-  </si>
-  <si>
-    <t>doc_Claim</t>
-  </si>
-  <si>
-    <t>Resource type to carry information regarding reason for requesting  1) attachments to support claim submission, medical necessity and other reasons for attachments between payers and providers, and 2) additional information to support prior authorization requests.</t>
-  </si>
-  <si>
-    <t>!http://hl7.org/fhir/us/davinci-hrex/StructureDefinition/hrex-coverage</t>
-  </si>
-  <si>
-    <t>* Required resource type to request and fetch clinical information from data source
-* There **SHOULD** be a reason stated in `Task.statusReason` by the Data-Source-Server when the status is updated to 'failed', 'refused', 'cancelled' or 'held'</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/index.html</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-hrex/2020Sep/index.html</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/CapabilityStatement-us-core-server.html</t>
+    <t>1. For general security consideration refer to the FHIR [Security and Privacy Considerations](http://build.fhir.org/secpriv-module.html). 
+1. For security considerations specific to this guide refer to the [Security and Privacy](security.html) section.</t>
+  </si>
+  <si>
+    <t>Data Source Server CapabilityStatement</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-cdex/CapabilityStatement/data-source-server</t>
   </si>
 </sst>
 </file>
@@ -1026,7 +1033,7 @@
         <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C2" s="1"/>
     </row>
@@ -1035,7 +1042,7 @@
         <v>81</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1080,7 +1087,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B9" s="1" t="b">
         <v>1</v>
@@ -2318,8 +2325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="A8" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2349,7 +2356,7 @@
         <v>78</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>97</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2365,7 +2372,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -2373,7 +2380,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="207.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2381,7 +2388,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>99</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2389,34 +2396,34 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>100</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B11" s="17"/>
     </row>
     <row r="12" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -2426,17 +2433,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD2C781A-6E7A-BF4B-91B6-0E7EC88583AE}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="1"/>
     <col min="2" max="2" width="13.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" style="1" customWidth="1"/>
     <col min="5" max="5" width="48.83203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="16.6640625" style="1" customWidth="1"/>
@@ -2445,16 +2452,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>87</v>
@@ -2468,15 +2475,32 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>126</v>
+        <v>153</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>154</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="B3" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2504,7 +2528,7 @@
         <v>18</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>87</v>
@@ -2515,13 +2539,13 @@
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>89</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -2529,13 +2553,13 @@
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>122</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>52</v>
@@ -2550,7 +2574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -2582,28 +2606,28 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -2614,33 +2638,33 @@
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>144</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>52</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -2804,39 +2828,39 @@
         <v>73</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="W1" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="Y1" s="4" t="s">
         <v>135</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="81" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D2" s="10"/>
     </row>
     <row r="3" spans="1:25" ht="80" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="32" x14ac:dyDescent="0.2">
@@ -2847,18 +2871,18 @@
         <v>52</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:25" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -2948,10 +2972,10 @@
         <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>77</v>
@@ -2960,16 +2984,16 @@
         <v>91</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -3177,7 +3201,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>25</v>
@@ -3185,7 +3209,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>25</v>
@@ -3193,7 +3217,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>25</v>
@@ -3201,7 +3225,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Clarify how to find patient FHIR ID ([FHIR-38318]
</commit_message>
<xml_diff>
--- a/input/resources-spreadsheet/data-source-server.xlsx
+++ b/input/resources-spreadsheet/data-source-server.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/davinci-ecdx/input/resources-spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311EA4C3-1E0D-9542-8D2D-F156CFEC2000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BF98490-4497-4C4A-821A-FA13AACF0FE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="68260" yWindow="500" windowWidth="34140" windowHeight="28300" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="170">
   <si>
     <t>Element</t>
   </si>
@@ -603,6 +603,15 @@
   </si>
   <si>
     <t>doc_PractitionerRole</t>
+  </si>
+  <si>
+    <t>match</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://hl7.org/fhir/OperationDefinition/Patient-match</t>
+  </si>
+  <si>
+    <t>Used for discovery of the FHIR Patient.id by CDex Data Consumers</t>
   </si>
 </sst>
 </file>
@@ -797,7 +806,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1085,7 +1094,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2481,10 +2490,10 @@
   <dimension ref="A1:Y39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T12" sqref="T12"/>
+      <selection pane="bottomRight" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2684,7 +2693,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2713,6 +2722,23 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" t="s">
+        <v>169</v>
+      </c>
+    </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E3" s="1"/>
     </row>
@@ -2727,8 +2753,8 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F20" sqref="F20"/>
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
*Pre-Applied:** (Enhancement) update to support topic based subscriptions [FHIR-45628]
</commit_message>
<xml_diff>
--- a/input/resources-spreadsheet/data-source-server.xlsx
+++ b/input/resources-spreadsheet/data-source-server.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/davinci-ecdx/input/resources-spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D8CC29-F6D1-DC4D-B350-DFA73F2EE6DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25010230-2A2E-DB44-B9FA-70DC2E6836B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27020" yWindow="500" windowWidth="34140" windowHeight="28300" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27020" yWindow="500" windowWidth="34140" windowHeight="28300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -1774,7 +1774,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+    <sheetView zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
       <pane xSplit="6" ySplit="1" topLeftCell="G61" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2390,8 +2390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A70CC787-78D8-4AA0-BE43-37746049F77C}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fix link in publication request file and typo in capabilitystatements
</commit_message>
<xml_diff>
--- a/input/resources-spreadsheet/data-source-server.xlsx
+++ b/input/resources-spreadsheet/data-source-server.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/davinci-ecdx/input/resources-spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2E4A87-91D2-FF43-965D-1A84563FEEC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE73394-41FF-DD49-8CFC-4DCBCC94430E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="64420" yWindow="500" windowWidth="34140" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="64420" yWindow="500" windowWidth="34140" windowHeight="28300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -1224,7 +1224,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2441,8 +2441,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>